<commit_message>
atualizando relatorio psci.. e db
</commit_message>
<xml_diff>
--- a/LmStudio/Rag_bot/Management_files/TableSchema.xlsx
+++ b/LmStudio/Rag_bot/Management_files/TableSchema.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inmotionconsulting-my.sharepoint.com/personal/bc_inmotion_today/Documents/AI Projects/AI-CAC-V1.3/LmStudio/Rag_bot/Management_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_497E5174D77EAAF1064EFB62CAEC9930095B33E1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39AC2556-8276-4D82-8B64-57F8AA03B10F}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Instruction"/>
-    <sheet r:id="rId2" sheetId="2" name="Feedback"/>
-    <sheet r:id="rId3" sheetId="3" name="PatientExperienceExpert"/>
-    <sheet r:id="rId4" sheetId="4" name="HealthITProcessExpert"/>
-    <sheet r:id="rId5" sheetId="5" name="ClinicalPsychologist"/>
-    <sheet r:id="rId6" sheetId="6" name="CommunicationExpert"/>
-    <sheet r:id="rId7" sheetId="7" name="ManagerAndAdvisor"/>
+    <sheet name="Instruction" sheetId="1" r:id="rId1"/>
+    <sheet name="Feedback" sheetId="2" r:id="rId2"/>
+    <sheet name="PatientExperienceExpert" sheetId="3" r:id="rId3"/>
+    <sheet name="HealthITProcessExpert" sheetId="4" r:id="rId4"/>
+    <sheet name="ClinicalPsychologist" sheetId="5" r:id="rId5"/>
+    <sheet name="CommunicationExpert" sheetId="6" r:id="rId6"/>
+    <sheet name="ManagerAndAdvisor" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -168,15 +174,6 @@
   </si>
   <si>
     <t>Suggested_Approach_Clinical_Psychologist</t>
-  </si>
-  <si>
-    <t>- The patient exhibits profound emotional distress, characterized by feelings of hopelessness and disengagement. This indicates a significant decline in their mental well-being.</t>
-  </si>
-  <si>
-    <t>- Conduct an urgent assessment session focusing on suicidal ideation and immediate safety concerns. - Develop a crisis management plan, including regular check-ins, therapeutic interventions tailored for depression (e.g., CBT), and possibly involving family or close friends in supportive roles. Explore</t>
-  </si>
-  <si>
-    <t>-  Conduct an urgent assessment session focusing on suicidal ideation and immediate safety concerns. - Develop a crisis management plan, including regular check-ins, therapeutic interventions tailored for depression (e.g., CBT), and possibly involving family or close friends in supportive</t>
   </si>
   <si>
     <t>- The patient expresses frustration and confusion regarding communication with their doctor, indicating a negative emotional state due to perceived language barriers.</t>
@@ -740,13 +737,21 @@
       <t>, which will allow easy querying across all expert analyses for a given piece of patient feedback.</t>
     </r>
   </si>
+  <si>
+    <t>The patient is experiencing a sense of detachment, disinterest, and frustration with their progress.</t>
+  </si>
+  <si>
+    <t>Implement a supportive strategy that focuses on rebuilding interest in their evolution and improving their overall well-being</t>
+  </si>
+  <si>
+    <t>Schedule regular check-ins to monitor progress and provide ongoing support</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -780,6 +785,25 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -808,77 +832,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -889,10 +901,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -930,71 +942,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1022,7 +1034,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1045,11 +1057,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1058,13 +1070,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1074,7 +1086,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1083,7 +1095,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1092,7 +1104,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1100,10 +1112,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1168,7 +1180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1176,542 +1188,452 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="19" width="69.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="20" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="20" width="48.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="69.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="22.5">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A1" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A4" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="16"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5" customFormat="1" s="1">
-      <c r="A4" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="7" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="2" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A9" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="10" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A11" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="22.5">
-      <c r="A9" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="31.5" customFormat="1" s="1">
-      <c r="A12" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
+    </row>
+    <row r="12" spans="1:3" s="1" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A12" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A14" s="2" t="s">
+    <row r="16" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A17" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C15" s="2" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="19" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A19" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A16" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C16" s="2" t="s">
+    <row r="20" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="21" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A21" s="12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A17" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="16"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="22.5">
-      <c r="A19" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="16"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="16"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="31.5" customFormat="1" s="1">
-      <c r="A23" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="22" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="23" spans="1:3" s="1" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A23" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5" customFormat="1" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A26" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A27" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="18" t="s">
+      <c r="B27" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C26" s="6" t="s">
+    </row>
+    <row r="28" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A28" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A27" s="2" t="s">
+      <c r="B28" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C27" s="2" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="30" spans="1:3" ht="22.5" customHeight="1">
+      <c r="A30" s="11" t="s">
         <v>157</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A28" s="2" t="s">
+    <row r="31" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="32" spans="1:3" ht="19.5" customHeight="1">
+      <c r="A32" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="16"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="22.5">
-      <c r="A30" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="16"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="16"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="31.5" customFormat="1" s="1">
-      <c r="A34" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5" customFormat="1" s="1">
+    </row>
+    <row r="33" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="34" spans="1:3" s="1" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A34" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5" customFormat="1" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="16"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="16"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="16"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A44" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="40" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A40" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="42" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A42" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="44" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A44" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="16"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="16"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="16"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A55" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="51" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A51" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="53" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A53" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="55" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A55" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" customFormat="1" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="16"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="15"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="18.75" customHeight="1"/>
+    <row r="60" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A60" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A61" s="12"/>
+    </row>
+    <row r="62" spans="1:3" ht="18.75" customHeight="1">
+      <c r="A62" s="12" t="s">
+        <v>173</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1719,132 +1641,134 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="5" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="38.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="19.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
-      <c r="A4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1853,7 +1777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1861,140 +1785,139 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="5" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="39.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="45.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="39.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="39.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="23.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="39.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C2" s="4">
         <v>-1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C3" s="4">
         <v>-0.5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C5" s="4">
         <v>0.8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C7" s="4">
         <v>-0.25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E8" s="4"/>
     </row>
@@ -2004,7 +1927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2012,135 +1935,132 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="5" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="40.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="68.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="56.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="68.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="23.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="8"/>
+        <v>69</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="8"/>
+        <v>72</v>
+      </c>
       <c r="D3" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>82</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="8"/>
+        <v>84</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>88</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2149,23 +2069,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="5" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="37.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="37.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="46.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="23.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2179,102 +2100,102 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>174</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>48</v>
+        <v>175</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2283,7 +2204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2291,16 +2212,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="5" width="24.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="45.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="39.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="47.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="44.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="24.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2317,7 +2238,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2334,7 +2255,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2351,7 +2272,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2366,7 +2287,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:5" ht="18.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -2381,7 +2302,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2396,7 +2317,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -2413,7 +2334,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -2434,7 +2355,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2442,14 +2363,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="5" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="32.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="39.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2460,7 +2381,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -2471,7 +2392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2482,7 +2403,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -2491,7 +2412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -2500,7 +2421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2509,7 +2430,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:3" ht="18.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -2520,7 +2441,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:3" ht="18.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>

</xml_diff>